<commit_message>
wireframes y flujos de interaccion
wireframes y flujos de interaccion, interfaz chat bot
</commit_message>
<xml_diff>
--- a/data/seguimiento_clientes_actualizado.xlsx
+++ b/data/seguimiento_clientes_actualizado.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-08-16 14:46:27</t>
+          <t>2025-08-16 17:22:42</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-08-16 14:46:27</t>
+          <t>2025-08-16 17:22:42</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-08-16 14:46:27</t>
+          <t>2025-08-16 17:22:42</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-08-16 14:46:27</t>
+          <t>2025-08-16 17:22:42</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-08-16 14:46:27</t>
+          <t>2025-08-16 17:22:42</t>
         </is>
       </c>
     </row>

</xml_diff>